<commit_message>
add profit/loss ratio for types:
</commit_message>
<xml_diff>
--- a/finance/calculator.xlsx
+++ b/finance/calculator.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sun_xo/learn/py/finance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF9AFC8-0533-E943-ACD5-0D24CE9F189E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B870A8-AD07-4548-A98D-05083CF8F36E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="500" windowWidth="22060" windowHeight="13620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="13620" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="复利" sheetId="2" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="网格" sheetId="7" r:id="rId5"/>
     <sheet name="期权" sheetId="4" r:id="rId6"/>
     <sheet name="房产计算" sheetId="1" r:id="rId7"/>
+    <sheet name="贝叶斯" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="threashold" localSheetId="2">指数阈值!$A$1:$H$59</definedName>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="497">
   <si>
     <t>Fv = Pv (1 + i) ^ n</t>
   </si>
@@ -1340,9 +1341,6 @@
     <t>委托金额(元)</t>
   </si>
   <si>
-    <t>https://legulegu.com/stockdata/sw-industry?industryCode=801193.SI</t>
-  </si>
-  <si>
     <t>ETF网格</t>
   </si>
   <si>
@@ -1368,18 +1366,229 @@
   </si>
   <si>
     <t>P下沿</t>
+  </si>
+  <si>
+    <t>委托股数(股)</t>
+  </si>
+  <si>
+    <t>SH510310</t>
+  </si>
+  <si>
+    <t>legulegu.com/stockdata/sw-industry?industryCode=801193.SI</t>
+  </si>
+  <si>
+    <t>指数</t>
+  </si>
+  <si>
+    <t>legulegu.com/stockdata/hs300-pb</t>
+  </si>
+  <si>
+    <t>即时卖1价</t>
+  </si>
+  <si>
+    <t>即时买1价</t>
+  </si>
+  <si>
+    <t>万顺转债</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>star</t>
+  </si>
+  <si>
+    <t>threshold</t>
+  </si>
+  <si>
+    <t>sh00985</t>
+  </si>
+  <si>
+    <t>base</t>
+  </si>
+  <si>
+    <t>搜特转债</t>
+  </si>
+  <si>
+    <t>累计股数</t>
+  </si>
+  <si>
+    <t>成本(元)</t>
+  </si>
+  <si>
+    <t>底部加仓</t>
+  </si>
+  <si>
+    <t>设条件单</t>
+  </si>
+  <si>
+    <t>执行后</t>
+  </si>
+  <si>
+    <t>改委托股数</t>
+  </si>
+  <si>
+    <t>10 -&gt; 30</t>
+  </si>
+  <si>
+    <t>(30-10)*4</t>
+  </si>
+  <si>
+    <t>&lt; 160 买80</t>
+  </si>
+  <si>
+    <t>p(B)=p(B|A)p(A)+p(B|Ᾱ)p(Ᾱ)</t>
+  </si>
+  <si>
+    <t>其中Ᾱ和A互斥，p(Ᾱ)=1-p(A)</t>
+  </si>
+  <si>
+    <t>p(B|A)*p(A)代表A,B同时发生</t>
+  </si>
+  <si>
+    <t>全概率公式</t>
+  </si>
+  <si>
+    <t>事件A发生的先验概率
+p(A)</t>
+  </si>
+  <si>
+    <t>事件A不发生
+的先验概率 
+p(Ᾱ) = 1 - p(A)</t>
+  </si>
+  <si>
+    <t>事件A发生时事件B发生的概率
+p (B|A)</t>
+  </si>
+  <si>
+    <t>事件A未发生时事件B发生的概率
+p(B|Ᾱ)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">事件B发生的概率
+p(B) = 
+p(B|A)p(A)+p(B|Ᾱ)p(Ᾱ) </t>
+  </si>
+  <si>
+    <t>事件A发生的后验概率
+p(A|B) =
+p(B|A)p(A)/p(B)</t>
+  </si>
+  <si>
+    <t>雍和宫灵验
+的先验概率</t>
+  </si>
+  <si>
+    <t>雍和宫不灵
+的先验概率</t>
+  </si>
+  <si>
+    <t>雍和宫灵验时
+某甲的升职概率</t>
+  </si>
+  <si>
+    <t>雍和宫不灵时
+某甲的升职概率</t>
+  </si>
+  <si>
+    <t>某甲的升职概率</t>
+  </si>
+  <si>
+    <t>雍和宫灵验的后验概率</t>
+  </si>
+  <si>
+    <t>0.15 -&gt; 0.22</t>
+  </si>
+  <si>
+    <t>某甲祈福后升职成功后雍和宫灵验的概率</t>
+  </si>
+  <si>
+    <t>某乙祈福后升职失败后雍和宫灵验的概率</t>
+  </si>
+  <si>
+    <t>雍和宫灵验时
+某乙不升职概率</t>
+  </si>
+  <si>
+    <t>雍和宫不灵时
+某乙不升职概率</t>
+  </si>
+  <si>
+    <t>0.22 -&gt; 0.10</t>
+  </si>
+  <si>
+    <t>携带HIV的先验概率</t>
+  </si>
+  <si>
+    <t>检测HIV为阳性的概率</t>
+  </si>
+  <si>
+    <t>不携带HIV的先验概率</t>
+  </si>
+  <si>
+    <t>检测为阳性后携带HIV的概率(后验概率)</t>
+  </si>
+  <si>
+    <t>携带者检测HIV为阳性的概率</t>
+  </si>
+  <si>
+    <t>非携带者检测为阳性的概率</t>
+  </si>
+  <si>
+    <t>案例1: 雍和宫灵验吗 - 事件A: 雍和宫灵验 事件B: 祈福后升职成功或失败</t>
+  </si>
+  <si>
+    <t>案例2: 某人检测HIV阳性 - 事件A: 携带HIV 事件B: 检测HIV阳性</t>
+  </si>
+  <si>
+    <t>第1次检测HIV阳性</t>
+  </si>
+  <si>
+    <t>第2次检测HIV阳性</t>
+  </si>
+  <si>
+    <t>某乙的不升职概率</t>
+  </si>
+  <si>
+    <t>案例3: 抓特务 - 事件A: 某人是间谍，事件B: 某人有嫌疑</t>
+  </si>
+  <si>
+    <t>某人是特务的先验概率</t>
+  </si>
+  <si>
+    <t>某人不是特务的先验概率</t>
+  </si>
+  <si>
+    <t>某人是特务且被怀疑的概率(真阳性)</t>
+  </si>
+  <si>
+    <t>某人不是特务却被怀疑的概率(假阳性)</t>
+  </si>
+  <si>
+    <t>某人被怀疑的概率</t>
+  </si>
+  <si>
+    <t>怀疑属实的概率(后验概率)</t>
+  </si>
+  <si>
+    <t>第一次被怀疑</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000000"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1408,6 +1617,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1432,11 +1649,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -1469,8 +1687,13 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -2083,10 +2306,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1488808B-A158-284F-9930-D604D6952601}">
-  <dimension ref="A3:F39"/>
+  <dimension ref="A3:F47"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="108" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView topLeftCell="A10" zoomScale="108" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2512,35 +2735,122 @@
         <v>4047.1092455742</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B39">
         <f>1657.7 * 1.1^(2021-2011) * (1+(12-1)/120) / 0.8^(5-4)</f>
         <v>5867.2264663553979</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>445</v>
+      </c>
+      <c r="B41">
+        <v>1657.7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>440</v>
+      </c>
+      <c r="B42">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>441</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>442</v>
+      </c>
+      <c r="B44">
+        <v>5</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
+      <c r="D44">
+        <v>3</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>443</v>
+      </c>
+      <c r="B45" s="18">
+        <f>$B$41 * 1.1^($B$42-2011) * (1+($B$43-1)/120) / 0.8^(5-B44)</f>
+        <v>4729.6115637185512</v>
+      </c>
+      <c r="C45" s="18">
+        <f t="shared" ref="C45:F45" si="14">$B$41 * 1.1^($B$42-2011) * (1+($B$43-1)/120) / 0.8^(5-C44)</f>
+        <v>5912.0144546481888</v>
+      </c>
+      <c r="D45" s="18">
+        <f t="shared" si="14"/>
+        <v>7390.0180683102344</v>
+      </c>
+      <c r="E45" s="18">
+        <f t="shared" si="14"/>
+        <v>9237.5225853877928</v>
+      </c>
+      <c r="F45" s="18">
+        <f t="shared" si="14"/>
+        <v>11546.903231734739</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>444</v>
+      </c>
+      <c r="B46">
+        <v>5568</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B47" s="24">
+        <f>(B45-$B$46)/$B$46</f>
+        <v>-0.15057263582640962</v>
+      </c>
+      <c r="C47" s="24">
+        <f>(C45-$B$46)/$B$46</f>
+        <v>6.1784205216987929E-2</v>
       </c>
     </row>
   </sheetData>
@@ -4150,7 +4460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14035F00-6F61-2846-A9B1-038887E13D80}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -4424,15 +4734,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEDC7B8B-DB21-EB49-B4A8-8BEBC5ED15A7}">
-  <dimension ref="A2:L51"/>
+  <dimension ref="A2:M79"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.83203125" bestFit="1" customWidth="1"/>
@@ -5008,7 +5318,7 @@
         <v>380</v>
       </c>
       <c r="F28" t="s">
-        <v>417</v>
+        <v>432</v>
       </c>
       <c r="G28" t="s">
         <v>383</v>
@@ -5068,320 +5378,1034 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>407</v>
-      </c>
-      <c r="B32" t="s">
-        <v>423</v>
-      </c>
-      <c r="G32" t="s">
-        <v>425</v>
-      </c>
+      <c r="B32" s="23"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>435</v>
+      </c>
+      <c r="B33" t="s">
+        <v>425</v>
+      </c>
+      <c r="C33" t="s">
+        <v>428</v>
+      </c>
+      <c r="D33" t="s">
         <v>426</v>
       </c>
-      <c r="B33" t="s">
+      <c r="E33" t="s">
+        <v>427</v>
+      </c>
+      <c r="F33" t="s">
         <v>429</v>
       </c>
-      <c r="C33" t="s">
-        <v>427</v>
-      </c>
-      <c r="D33" t="s">
-        <v>428</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="G33" t="s">
         <v>430</v>
       </c>
-      <c r="F33" t="s">
+      <c r="H33" t="s">
         <v>431</v>
       </c>
-      <c r="G33" t="s">
-        <v>432</v>
-      </c>
-      <c r="H33" t="s">
+      <c r="I33" t="s">
         <v>410</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34">
+      <c r="A34" t="s">
+        <v>407</v>
+      </c>
+      <c r="B34">
         <v>1.1759999999999999</v>
       </c>
-      <c r="B34">
+      <c r="C34" s="22">
         <v>1.79</v>
       </c>
-      <c r="C34">
+      <c r="D34" s="22">
         <v>2</v>
       </c>
-      <c r="D34">
+      <c r="E34" s="22">
         <v>1.5</v>
       </c>
-      <c r="E34" s="21">
-        <f>A34/B34</f>
+      <c r="F34" s="22">
+        <f>B34/C34</f>
         <v>0.65698324022346366</v>
       </c>
-      <c r="F34" s="21">
-        <f>C34*E34</f>
+      <c r="G34" s="22">
+        <f>D34*F34</f>
         <v>1.3139664804469273</v>
       </c>
-      <c r="G34" s="21">
-        <f>D34*E34</f>
+      <c r="H34" s="22">
+        <f>E34*F34</f>
         <v>0.98547486033519549</v>
       </c>
-      <c r="H34" s="21">
-        <f>(F34-G34)/10</f>
+      <c r="I34" s="22">
+        <f>(G34-H34)/10</f>
         <v>3.2849162011173182E-2</v>
+      </c>
+      <c r="J34" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>379</v>
-      </c>
-      <c r="B35" t="s">
-        <v>392</v>
-      </c>
-      <c r="C35" t="s">
-        <v>393</v>
-      </c>
-      <c r="D35" t="s">
-        <v>421</v>
-      </c>
-      <c r="E35" t="s">
-        <v>380</v>
-      </c>
-      <c r="F35" t="s">
-        <v>417</v>
-      </c>
-      <c r="G35" t="s">
-        <v>383</v>
-      </c>
-      <c r="H35" t="s">
-        <v>387</v>
-      </c>
-      <c r="I35" t="s">
-        <v>390</v>
+        <v>230</v>
+      </c>
+      <c r="B35">
+        <v>2.2919999999999998</v>
+      </c>
+      <c r="C35" s="22">
+        <v>1.58</v>
+      </c>
+      <c r="D35" s="22">
+        <v>1.78</v>
+      </c>
+      <c r="E35" s="22">
+        <v>1.4</v>
+      </c>
+      <c r="F35" s="22">
+        <f>B35/C35</f>
+        <v>1.4506329113924048</v>
+      </c>
+      <c r="G35" s="22">
+        <f>D35*F35</f>
+        <v>2.5821265822784807</v>
+      </c>
+      <c r="H35" s="22">
+        <f>E35*F35</f>
+        <v>2.0308860759493665</v>
+      </c>
+      <c r="I35" s="22">
+        <f>(G35-H35)/10</f>
+        <v>5.5124050632911412E-2</v>
       </c>
       <c r="J35" t="s">
-        <v>382</v>
-      </c>
-      <c r="K35" t="s">
-        <v>386</v>
-      </c>
-      <c r="L35" t="s">
-        <v>388</v>
+        <v>436</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="21"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="22"/>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E37" s="21"/>
-      <c r="F37" s="21"/>
-      <c r="G37" s="21"/>
-      <c r="H37" s="21"/>
+      <c r="A37" t="s">
+        <v>186</v>
+      </c>
+      <c r="B37">
+        <v>1.51</v>
+      </c>
+      <c r="C37" s="22">
+        <v>10.49</v>
+      </c>
+      <c r="D37" s="22">
+        <v>9.5</v>
+      </c>
+      <c r="E37" s="22">
+        <v>12.5</v>
+      </c>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22">
+        <f>B37*C37/D37</f>
+        <v>1.6673578947368421</v>
+      </c>
+      <c r="H37" s="22">
+        <f>B37*C37/E37</f>
+        <v>1.2671920000000001</v>
+      </c>
+      <c r="I37" s="22"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E38" s="22"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>414</v>
+        <v>379</v>
       </c>
       <c r="B39" t="s">
-        <v>413</v>
+        <v>392</v>
       </c>
       <c r="C39" t="s">
-        <v>408</v>
+        <v>393</v>
       </c>
       <c r="D39" t="s">
-        <v>409</v>
+        <v>421</v>
       </c>
       <c r="E39" t="s">
-        <v>410</v>
+        <v>380</v>
+      </c>
+      <c r="F39" t="s">
+        <v>432</v>
+      </c>
+      <c r="G39" t="s">
+        <v>383</v>
+      </c>
+      <c r="H39" t="s">
+        <v>387</v>
+      </c>
+      <c r="I39" t="s">
+        <v>390</v>
+      </c>
+      <c r="J39" t="s">
+        <v>382</v>
+      </c>
+      <c r="K39" t="s">
+        <v>386</v>
+      </c>
+      <c r="L39" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>407</v>
-      </c>
-      <c r="B40">
-        <v>512880</v>
-      </c>
-      <c r="C40">
-        <v>1.3240000000000001</v>
-      </c>
-      <c r="D40">
-        <v>1.02</v>
-      </c>
-      <c r="E40">
-        <v>0.03</v>
+        <v>424</v>
+      </c>
+      <c r="B40" s="22">
+        <f>H34</f>
+        <v>0.98547486033519549</v>
+      </c>
+      <c r="C40" s="22">
+        <f>G34</f>
+        <v>1.3139664804469273</v>
+      </c>
+      <c r="D40" s="22">
+        <f>C40</f>
+        <v>1.3139664804469273</v>
+      </c>
+      <c r="E40" s="21" t="s">
+        <v>381</v>
+      </c>
+      <c r="F40" s="18">
+        <v>1000</v>
+      </c>
+      <c r="G40" s="22">
+        <f>-I34</f>
+        <v>-3.2849162011173182E-2</v>
+      </c>
+      <c r="H40" s="22">
+        <f>-G40/10</f>
+        <v>3.2849162011173182E-3</v>
+      </c>
+      <c r="I40" s="21" t="s">
+        <v>391</v>
+      </c>
+      <c r="J40" s="22">
+        <f>I34</f>
+        <v>3.2849162011173182E-2</v>
+      </c>
+      <c r="K40" s="22">
+        <f>-J40/10</f>
+        <v>-3.2849162011173182E-3</v>
+      </c>
+      <c r="L40" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>411</v>
-      </c>
-      <c r="B41">
-        <v>512910</v>
-      </c>
-      <c r="C41">
-        <v>1.6720699999999999</v>
-      </c>
-      <c r="D41">
-        <v>1.27864</v>
-      </c>
-      <c r="E41">
-        <v>3.934E-2</v>
+        <v>433</v>
+      </c>
+      <c r="B41" s="22">
+        <f>H35</f>
+        <v>2.0308860759493665</v>
+      </c>
+      <c r="C41" s="22">
+        <f>G35</f>
+        <v>2.5821265822784807</v>
+      </c>
+      <c r="D41" s="22">
+        <f>C41</f>
+        <v>2.5821265822784807</v>
+      </c>
+      <c r="E41" s="21" t="s">
+        <v>381</v>
+      </c>
+      <c r="F41" s="18">
+        <v>1000</v>
+      </c>
+      <c r="G41" s="22">
+        <f>-I35</f>
+        <v>-5.5124050632911412E-2</v>
+      </c>
+      <c r="H41" s="22">
+        <f>-G41/10</f>
+        <v>5.5124050632911412E-3</v>
+      </c>
+      <c r="I41" s="21" t="s">
+        <v>391</v>
+      </c>
+      <c r="J41" s="22">
+        <f>I35</f>
+        <v>5.5124050632911412E-2</v>
+      </c>
+      <c r="K41" s="22">
+        <f>-J41/10</f>
+        <v>-5.5124050632911412E-3</v>
+      </c>
+      <c r="L41" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>412</v>
-      </c>
-      <c r="B42">
-        <v>159905</v>
-      </c>
-      <c r="C42">
-        <v>2.8639999999999999</v>
-      </c>
-      <c r="D42">
-        <v>2.129</v>
-      </c>
-      <c r="E42">
-        <v>7.2999999999999995E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>230</v>
-      </c>
-      <c r="B43">
-        <v>510310</v>
-      </c>
-      <c r="C43">
-        <v>2.6549999999999998</v>
-      </c>
-      <c r="D43">
-        <v>2.0550000000000002</v>
-      </c>
-      <c r="E43">
-        <v>0.06</v>
+      <c r="B42" s="22"/>
+      <c r="C42" s="22"/>
+      <c r="D42" s="22"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="22"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="22"/>
+      <c r="K42" s="22"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>414</v>
+      </c>
+      <c r="B44" t="s">
+        <v>413</v>
+      </c>
+      <c r="C44" t="s">
+        <v>408</v>
+      </c>
+      <c r="D44" t="s">
+        <v>409</v>
+      </c>
+      <c r="E44" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>420</v>
+        <v>407</v>
+      </c>
+      <c r="B45">
+        <v>512880</v>
+      </c>
+      <c r="C45">
+        <v>1.3240000000000001</v>
+      </c>
+      <c r="D45">
+        <v>1.02</v>
+      </c>
+      <c r="E45">
+        <v>0.03</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
+        <v>411</v>
+      </c>
+      <c r="B46">
+        <v>512910</v>
+      </c>
+      <c r="C46">
+        <v>1.6720699999999999</v>
+      </c>
+      <c r="D46">
+        <v>1.27864</v>
+      </c>
+      <c r="E46">
+        <v>3.934E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>412</v>
+      </c>
+      <c r="B47">
+        <v>159905</v>
+      </c>
+      <c r="C47">
+        <v>2.8639999999999999</v>
+      </c>
+      <c r="D47">
+        <v>2.129</v>
+      </c>
+      <c r="E47">
+        <v>7.2999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>230</v>
+      </c>
+      <c r="B48">
+        <v>510310</v>
+      </c>
+      <c r="C48">
+        <v>2.6549999999999998</v>
+      </c>
+      <c r="D48">
+        <v>2.0550000000000002</v>
+      </c>
+      <c r="E48">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
         <v>407</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B51" t="s">
         <v>392</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C51" t="s">
         <v>393</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D51" t="s">
         <v>421</v>
       </c>
-      <c r="E46" t="s">
+      <c r="E51" t="s">
         <v>380</v>
       </c>
-      <c r="F46" s="20" t="s">
+      <c r="F51" s="20" t="s">
         <v>422</v>
       </c>
-      <c r="G46" t="s">
+      <c r="G51" t="s">
         <v>383</v>
       </c>
-      <c r="H46" t="s">
+      <c r="H51" t="s">
         <v>387</v>
       </c>
-      <c r="I46" t="s">
+      <c r="I51" t="s">
         <v>390</v>
       </c>
-      <c r="J46" t="s">
+      <c r="J51" t="s">
         <v>382</v>
       </c>
-      <c r="K46" t="s">
+      <c r="K51" t="s">
         <v>386</v>
       </c>
-      <c r="L46" t="s">
+      <c r="L51" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A47">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A52">
         <v>512880</v>
       </c>
-      <c r="B47">
+      <c r="B52">
         <v>1.02</v>
       </c>
-      <c r="C47">
+      <c r="C52">
         <v>1.32</v>
       </c>
-      <c r="D47">
+      <c r="D52">
         <v>1.32</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E52" t="s">
         <v>381</v>
       </c>
-      <c r="F47">
+      <c r="F52">
         <v>5000</v>
       </c>
-      <c r="G47">
+      <c r="G52">
         <v>-0.03</v>
       </c>
-      <c r="H47">
+      <c r="H52">
         <v>1E-3</v>
       </c>
-      <c r="I47" t="s">
+      <c r="I52" t="s">
         <v>391</v>
       </c>
-      <c r="J47">
+      <c r="J52">
         <v>0.03</v>
       </c>
-      <c r="K47">
+      <c r="K52">
         <v>-1E-3</v>
       </c>
-      <c r="L47" t="s">
+      <c r="L52" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>415</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B55" t="s">
         <v>416</v>
       </c>
-      <c r="C50" s="20" t="s">
+      <c r="C55" s="20" t="s">
         <v>419</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D55" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A56">
         <v>1.3240000000000001</v>
       </c>
-      <c r="B51" s="5">
+      <c r="B56" s="5">
         <v>-0.01</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C56" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B57" s="5"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="H58" s="1"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>439</v>
+      </c>
+      <c r="B59">
+        <v>123012</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>355</v>
+      </c>
+      <c r="B60" t="s">
+        <v>374</v>
+      </c>
+      <c r="C60" t="s">
+        <v>417</v>
+      </c>
+      <c r="D60" t="s">
+        <v>447</v>
+      </c>
+      <c r="E60" t="s">
+        <v>375</v>
+      </c>
+      <c r="F60" t="s">
+        <v>448</v>
+      </c>
+      <c r="G60" t="s">
+        <v>384</v>
+      </c>
+      <c r="H60" t="s">
+        <v>385</v>
+      </c>
+      <c r="J60" t="s">
+        <v>449</v>
+      </c>
+      <c r="K60" t="s">
+        <v>417</v>
+      </c>
+      <c r="L60" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>0</v>
+      </c>
+      <c r="B61">
+        <v>200</v>
+      </c>
+      <c r="J61" t="s">
+        <v>450</v>
+      </c>
+      <c r="K61" t="s">
+        <v>455</v>
+      </c>
+      <c r="L61" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>1</v>
+      </c>
+      <c r="B62">
+        <v>190</v>
+      </c>
+      <c r="C62">
+        <v>30</v>
+      </c>
+      <c r="D62">
+        <f>C62*A62</f>
+        <v>30</v>
+      </c>
+      <c r="E62">
+        <f>B62*C62</f>
+        <v>5700</v>
+      </c>
+      <c r="F62">
+        <f>SUM($E$62:E62)</f>
+        <v>5700</v>
+      </c>
+      <c r="G62">
+        <f>B62*D62-F62</f>
+        <v>0</v>
+      </c>
+      <c r="H62" s="1">
+        <f>G62/F62</f>
+        <v>0</v>
+      </c>
+      <c r="J62" t="s">
+        <v>451</v>
+      </c>
+      <c r="K62" t="s">
+        <v>452</v>
+      </c>
+      <c r="L62">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>2</v>
+      </c>
+      <c r="B63">
+        <v>180</v>
+      </c>
+      <c r="C63">
+        <v>30</v>
+      </c>
+      <c r="D63">
+        <f t="shared" ref="D63:D65" si="7">C63*A63</f>
+        <v>60</v>
+      </c>
+      <c r="E63">
+        <f t="shared" ref="E63:E65" si="8">B63*C63</f>
+        <v>5400</v>
+      </c>
+      <c r="F63">
+        <f>SUM($E$62:E63)</f>
+        <v>11100</v>
+      </c>
+      <c r="G63">
+        <f t="shared" ref="G63:G65" si="9">B63*D63-F63</f>
+        <v>-300</v>
+      </c>
+      <c r="H63" s="1">
+        <f t="shared" ref="H63:H65" si="10">G63/F63</f>
+        <v>-2.7027027027027029E-2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>3</v>
+      </c>
+      <c r="B64">
+        <v>170</v>
+      </c>
+      <c r="C64">
+        <v>30</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="7"/>
+        <v>90</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="8"/>
+        <v>5100</v>
+      </c>
+      <c r="F64">
+        <f>SUM($E$62:E64)</f>
+        <v>16200</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="9"/>
+        <v>-900</v>
+      </c>
+      <c r="H64" s="1">
+        <f t="shared" si="10"/>
+        <v>-5.5555555555555552E-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>4</v>
+      </c>
+      <c r="B65">
+        <v>160</v>
+      </c>
+      <c r="C65">
+        <v>30</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="7"/>
+        <v>120</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="8"/>
+        <v>4800</v>
+      </c>
+      <c r="F65">
+        <f>SUM($E$62:E65)</f>
+        <v>21000</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="9"/>
+        <v>-1800</v>
+      </c>
+      <c r="H65" s="1">
+        <f t="shared" si="10"/>
+        <v>-8.5714285714285715E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H66" s="1"/>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>446</v>
+      </c>
+      <c r="B67">
+        <v>128100</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>355</v>
+      </c>
+      <c r="B68" t="s">
+        <v>374</v>
+      </c>
+      <c r="C68" t="s">
+        <v>417</v>
+      </c>
+      <c r="D68" t="s">
+        <v>447</v>
+      </c>
+      <c r="E68" t="s">
+        <v>375</v>
+      </c>
+      <c r="F68" t="s">
+        <v>448</v>
+      </c>
+      <c r="G68" t="s">
+        <v>384</v>
+      </c>
+      <c r="H68" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>0</v>
+      </c>
+      <c r="B69">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>1</v>
+      </c>
+      <c r="B70">
+        <v>115</v>
+      </c>
+      <c r="C70">
+        <v>30</v>
+      </c>
+      <c r="D70">
+        <f>SUM($C$70:C70)</f>
+        <v>30</v>
+      </c>
+      <c r="E70">
+        <f>B70*C70</f>
+        <v>3450</v>
+      </c>
+      <c r="F70">
+        <f>SUM($E$70:E70)</f>
+        <v>3450</v>
+      </c>
+      <c r="G70">
+        <f>B70*D70-F70</f>
+        <v>0</v>
+      </c>
+      <c r="H70" s="1">
+        <f>G70/F70</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>2</v>
+      </c>
+      <c r="B71">
+        <v>110</v>
+      </c>
+      <c r="C71">
+        <v>30</v>
+      </c>
+      <c r="D71">
+        <f>SUM($C$70:C71)</f>
+        <v>60</v>
+      </c>
+      <c r="E71">
+        <f t="shared" ref="E71:E73" si="11">B71*C71</f>
+        <v>3300</v>
+      </c>
+      <c r="F71">
+        <f>SUM($E$70:E71)</f>
+        <v>6750</v>
+      </c>
+      <c r="G71">
+        <f t="shared" ref="G71:G73" si="12">B71*D71-F71</f>
+        <v>-150</v>
+      </c>
+      <c r="H71" s="1">
+        <f t="shared" ref="H71:H73" si="13">G71/F71</f>
+        <v>-2.2222222222222223E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>3</v>
+      </c>
+      <c r="B72">
+        <v>105</v>
+      </c>
+      <c r="C72">
+        <v>30</v>
+      </c>
+      <c r="D72">
+        <f>SUM($C$70:C72)</f>
+        <v>90</v>
+      </c>
+      <c r="E72">
+        <f t="shared" si="11"/>
+        <v>3150</v>
+      </c>
+      <c r="F72">
+        <f>SUM($E$70:E72)</f>
+        <v>9900</v>
+      </c>
+      <c r="G72">
+        <f t="shared" si="12"/>
+        <v>-450</v>
+      </c>
+      <c r="H72" s="1">
+        <f t="shared" si="13"/>
+        <v>-4.5454545454545456E-2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>4</v>
+      </c>
+      <c r="B73">
+        <v>100</v>
+      </c>
+      <c r="C73">
+        <v>30</v>
+      </c>
+      <c r="D73">
+        <f>SUM($C$70:C73)</f>
+        <v>120</v>
+      </c>
+      <c r="E73">
+        <f t="shared" si="11"/>
+        <v>3000</v>
+      </c>
+      <c r="F73">
+        <f>SUM($E$70:E73)</f>
+        <v>12900</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="12"/>
+        <v>-900</v>
+      </c>
+      <c r="H73" s="1">
+        <f t="shared" si="13"/>
+        <v>-6.9767441860465115E-2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H74" s="1"/>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>379</v>
+      </c>
+      <c r="B76" t="s">
+        <v>392</v>
+      </c>
+      <c r="C76" t="s">
+        <v>393</v>
+      </c>
+      <c r="D76" t="s">
+        <v>421</v>
+      </c>
+      <c r="E76" t="s">
+        <v>380</v>
+      </c>
+      <c r="F76" t="s">
+        <v>432</v>
+      </c>
+      <c r="G76" t="s">
+        <v>382</v>
+      </c>
+      <c r="H76" t="s">
+        <v>386</v>
+      </c>
+      <c r="I76" t="s">
+        <v>388</v>
+      </c>
+      <c r="J76" t="s">
+        <v>383</v>
+      </c>
+      <c r="K76" t="s">
+        <v>387</v>
+      </c>
+      <c r="L76" t="s">
+        <v>390</v>
+      </c>
+      <c r="M76" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>110038</v>
+      </c>
+      <c r="B77">
+        <v>115</v>
+      </c>
+      <c r="C77">
+        <v>155</v>
+      </c>
+      <c r="D77">
+        <v>155</v>
+      </c>
+      <c r="E77" t="s">
+        <v>381</v>
+      </c>
+      <c r="F77">
+        <v>10</v>
+      </c>
+      <c r="G77">
+        <v>10</v>
+      </c>
+      <c r="H77">
+        <f>-G77/10</f>
+        <v>-1</v>
+      </c>
+      <c r="I77" t="s">
+        <v>438</v>
+      </c>
+      <c r="J77">
+        <v>-10</v>
+      </c>
+      <c r="K77">
+        <f>-J77/10</f>
+        <v>1</v>
+      </c>
+      <c r="L77" t="s">
+        <v>437</v>
+      </c>
+      <c r="M77">
+        <f t="shared" ref="M77:M79" si="14">(B77+C77-10)*2*10</f>
+        <v>5200</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>123012</v>
+      </c>
+      <c r="B78">
+        <v>160</v>
+      </c>
+      <c r="C78">
+        <v>200</v>
+      </c>
+      <c r="D78">
+        <v>200</v>
+      </c>
+      <c r="E78" t="s">
+        <v>381</v>
+      </c>
+      <c r="F78">
+        <v>10</v>
+      </c>
+      <c r="G78">
+        <v>10</v>
+      </c>
+      <c r="H78">
+        <f>-G78/10</f>
+        <v>-1</v>
+      </c>
+      <c r="I78" t="s">
+        <v>438</v>
+      </c>
+      <c r="J78">
+        <v>-10</v>
+      </c>
+      <c r="K78">
+        <f>-J78/10</f>
+        <v>1</v>
+      </c>
+      <c r="L78" t="s">
+        <v>437</v>
+      </c>
+      <c r="M78">
+        <f t="shared" si="14"/>
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>128100</v>
+      </c>
+      <c r="B79">
+        <v>100</v>
+      </c>
+      <c r="C79">
+        <v>120</v>
+      </c>
+      <c r="D79">
+        <f>C79</f>
+        <v>120</v>
+      </c>
+      <c r="E79" t="s">
+        <v>381</v>
+      </c>
+      <c r="F79">
+        <v>30</v>
+      </c>
+      <c r="G79">
+        <v>5</v>
+      </c>
+      <c r="H79">
+        <f>-G79/10</f>
+        <v>-0.5</v>
+      </c>
+      <c r="I79" t="s">
+        <v>438</v>
+      </c>
+      <c r="J79">
+        <v>-5</v>
+      </c>
+      <c r="K79">
+        <f>-J79/10</f>
+        <v>0.5</v>
+      </c>
+      <c r="L79" t="s">
+        <v>437</v>
+      </c>
+      <c r="M79">
+        <f t="shared" si="14"/>
+        <v>4200</v>
       </c>
     </row>
   </sheetData>
@@ -6019,7 +7043,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A15" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -6401,4 +7425,319 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE5A4E00-D05A-8A48-9385-B4D2154494C1}">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="68" x14ac:dyDescent="0.2">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>460</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>461</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>462</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>463</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>464</v>
+      </c>
+      <c r="G6" s="11" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="25" t="s">
+        <v>484</v>
+      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>473</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>466</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>467</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>468</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>469</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>470</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>472</v>
+      </c>
+      <c r="B9">
+        <v>0.15</v>
+      </c>
+      <c r="C9">
+        <f>1-B9</f>
+        <v>0.85</v>
+      </c>
+      <c r="D9">
+        <v>0.8</v>
+      </c>
+      <c r="E9">
+        <v>0.5</v>
+      </c>
+      <c r="F9">
+        <f>B9*D9+C9*E9</f>
+        <v>0.54499999999999993</v>
+      </c>
+      <c r="G9" s="22">
+        <f>D9*B9/F9</f>
+        <v>0.22018348623853212</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>474</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>466</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>467</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>475</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>476</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>488</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>477</v>
+      </c>
+      <c r="B11" s="22">
+        <f>G9</f>
+        <v>0.22018348623853212</v>
+      </c>
+      <c r="C11" s="22">
+        <f>1-B11</f>
+        <v>0.77981651376146788</v>
+      </c>
+      <c r="D11">
+        <f>1-D9</f>
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="E11">
+        <f>1-E9</f>
+        <v>0.5</v>
+      </c>
+      <c r="F11" s="22">
+        <f>B11*D11+C11*E11</f>
+        <v>0.43394495412844036</v>
+      </c>
+      <c r="G11" s="22">
+        <f>B11*D11/F11</f>
+        <v>0.1014799154334038</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="11"/>
+      <c r="B12" s="22"/>
+      <c r="C12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="25" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11" t="s">
+        <v>478</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>480</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>482</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>483</v>
+      </c>
+      <c r="F14" t="s">
+        <v>479</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="11" t="s">
+        <v>486</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1E-4</v>
+      </c>
+      <c r="C15" s="5">
+        <f>1-B15</f>
+        <v>0.99990000000000001</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0.999</v>
+      </c>
+      <c r="E15" s="5">
+        <v>1E-4</v>
+      </c>
+      <c r="F15" s="5">
+        <f>B15*D15+C15*E15</f>
+        <v>1.9989000000000001E-4</v>
+      </c>
+      <c r="G15" s="5">
+        <f>B15*D15/F15</f>
+        <v>0.49977487618190003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="11" t="s">
+        <v>487</v>
+      </c>
+      <c r="B16" s="5">
+        <f>G15</f>
+        <v>0.49977487618190003</v>
+      </c>
+      <c r="C16" s="5">
+        <f>1-B16</f>
+        <v>0.50022512381809991</v>
+      </c>
+      <c r="D16" s="5">
+        <v>0.999</v>
+      </c>
+      <c r="E16" s="5">
+        <v>1E-4</v>
+      </c>
+      <c r="F16" s="5">
+        <f>B16*D16+C16*E16</f>
+        <v>0.4993251238180999</v>
+      </c>
+      <c r="G16" s="5">
+        <f>B16*D16/F16</f>
+        <v>0.99989981975671627</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="25" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11" t="s">
+        <v>490</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>491</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>492</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>493</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>494</v>
+      </c>
+      <c r="G19" s="11" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="11" t="s">
+        <v>496</v>
+      </c>
+      <c r="B20" s="5">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="C20" s="5">
+        <f>1-B20</f>
+        <v>0.99970000000000003</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.99</v>
+      </c>
+      <c r="E20" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="F20" s="5">
+        <f>B20*D20+C20*E20</f>
+        <v>5.0282E-2</v>
+      </c>
+      <c r="G20" s="5">
+        <f>B20*C20/F20</f>
+        <v>5.9645598822640304E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>